<commit_message>
Add test for JSONata, document limitation for binary mapping
</commit_message>
<xml_diff>
--- a/resources/script/mapping/sampleMapping/SampleMappings_11.xlsx
+++ b/resources/script/mapping/sampleMapping/SampleMappings_11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ck/work/git/cumulocity-dynamic-mapper/resources/script/mapping/sampleMapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2D5442-C9F6-5146-AF4E-F211A80AC13D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607789B0-DBE7-8B4A-B73D-0B7AA30EBD98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="76800" windowHeight="31500" xr2:uid="{B5E387B2-3E90-884E-B546-D827ECD68714}"/>
+    <workbookView xWindow="18600" yWindow="32760" windowWidth="34560" windowHeight="21580" xr2:uid="{B5E387B2-3E90-884E-B546-D827ECD68714}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1063,7 +1063,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1086,7 +1086,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1439,20 +1438,19 @@
   </sheetPr>
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="142" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="142" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="13"/>
-    <col min="2" max="2" width="18.83203125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="12"/>
+    <col min="2" max="2" width="18.83203125" style="12" customWidth="1"/>
     <col min="3" max="3" width="51.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="14"/>
+    <col min="4" max="4" width="10.83203125" style="13"/>
     <col min="5" max="5" width="46" style="1" customWidth="1"/>
     <col min="6" max="6" width="44" style="1" customWidth="1"/>
-    <col min="7" max="7" width="24.33203125" style="19" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="8"/>
+    <col min="7" max="7" width="24.33203125" style="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="28" x14ac:dyDescent="0.2">
@@ -1462,33 +1460,33 @@
       <c r="B1" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="17" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="182" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -1502,16 +1500,16 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="384" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -1525,16 +1523,16 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="182" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -1548,16 +1546,16 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="154" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -1571,16 +1569,16 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="182" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -1594,16 +1592,16 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="196" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -1617,16 +1615,16 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="4" t="s">
@@ -1640,16 +1638,16 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="154" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="4" t="s">
@@ -1663,16 +1661,16 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="196" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -1686,16 +1684,16 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="126" x14ac:dyDescent="0.2">
-      <c r="A11" s="9">
+      <c r="A11" s="8">
         <v>13</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>56</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -1709,16 +1707,16 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="112" x14ac:dyDescent="0.2">
-      <c r="A12" s="9">
+      <c r="A12" s="8">
         <v>14</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="2" t="s">
@@ -1732,16 +1730,16 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="140" x14ac:dyDescent="0.2">
-      <c r="A13" s="9">
+      <c r="A13" s="8">
         <v>15</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>56</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="2" t="s">
@@ -1755,16 +1753,16 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="98" x14ac:dyDescent="0.2">
-      <c r="A14" s="9">
+      <c r="A14" s="8">
         <v>17</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="9" t="s">
         <v>5</v>
       </c>
       <c r="E14" s="2" t="s">
@@ -1778,16 +1776,16 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="266" x14ac:dyDescent="0.2">
-      <c r="A15" s="9">
+      <c r="A15" s="8">
         <v>18</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>55</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E15" s="2" t="s">
@@ -1801,16 +1799,16 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="332" x14ac:dyDescent="0.2">
-      <c r="A16" s="9">
+      <c r="A16" s="8">
         <v>19</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>54</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E16" s="2" t="s">
@@ -1824,16 +1822,16 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="182" x14ac:dyDescent="0.2">
-      <c r="A17" s="9">
+      <c r="A17" s="8">
         <v>20</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="9" t="s">
         <v>27</v>
       </c>
       <c r="E17" s="2" t="s">
@@ -1847,16 +1845,16 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="112" x14ac:dyDescent="0.2">
-      <c r="A18" s="9">
+      <c r="A18" s="8">
         <v>21</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E18" s="2" t="s">
@@ -1870,16 +1868,16 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="210" x14ac:dyDescent="0.2">
-      <c r="A19" s="9">
+      <c r="A19" s="8">
         <v>23</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E19" s="2" t="s">
@@ -1893,16 +1891,16 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="140" x14ac:dyDescent="0.2">
-      <c r="A20" s="9">
+      <c r="A20" s="8">
         <v>24</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E20" s="2" t="s">
@@ -1916,16 +1914,16 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="252" x14ac:dyDescent="0.2">
-      <c r="A21" s="9">
+      <c r="A21" s="8">
         <v>25</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>54</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="2" t="s">
@@ -1939,16 +1937,16 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="168" x14ac:dyDescent="0.2">
-      <c r="A22" s="9">
+      <c r="A22" s="8">
         <v>26</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E22" s="2" t="s">
@@ -1962,16 +1960,16 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="196" x14ac:dyDescent="0.2">
-      <c r="A23" s="9">
+      <c r="A23" s="8">
         <v>27</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E23" s="2" t="s">
@@ -1985,16 +1983,16 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="224" x14ac:dyDescent="0.2">
-      <c r="A24" s="9">
+      <c r="A24" s="8">
         <v>51</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="10" t="s">
         <v>66</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E24" s="2" t="s">
@@ -2008,16 +2006,16 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="196" x14ac:dyDescent="0.2">
-      <c r="A25" s="9">
+      <c r="A25" s="8">
         <v>52</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="10" t="s">
         <v>66</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E25" s="2" t="s">
@@ -2031,16 +2029,16 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="210" x14ac:dyDescent="0.2">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="10" t="s">
         <v>66</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E26" s="2" t="s">
@@ -2054,7 +2052,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F29" s="17"/>
+      <c r="F29" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>

</xml_diff>